<commit_message>
new plots created by modal filter.
</commit_message>
<xml_diff>
--- a/sigGOterms.xlsx
+++ b/sigGOterms.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="0" windowWidth="25020" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="17040" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="First ver." sheetId="1" r:id="rId1"/>
+    <sheet name="Second ver." sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="290">
   <si>
     <t>organ</t>
   </si>
@@ -427,16 +428,494 @@
   </si>
   <si>
     <t>affected_groups</t>
+  </si>
+  <si>
+    <t>GO:0005521</t>
+  </si>
+  <si>
+    <t>GO:0006904</t>
+  </si>
+  <si>
+    <t>GO:0030863</t>
+  </si>
+  <si>
+    <t>GO:0030955</t>
+  </si>
+  <si>
+    <t>GO:0035097</t>
+  </si>
+  <si>
+    <t>GO:0043034</t>
+  </si>
+  <si>
+    <t>gorilla,monkey,orangutan</t>
+  </si>
+  <si>
+    <t>GO:0046513</t>
+  </si>
+  <si>
+    <t>orangutan,monkey</t>
+  </si>
+  <si>
+    <t>GO:0048813</t>
+  </si>
+  <si>
+    <t>GO:0051968</t>
+  </si>
+  <si>
+    <t>GO:0060337</t>
+  </si>
+  <si>
+    <t>GO:0060999</t>
+  </si>
+  <si>
+    <t>GO:0002026</t>
+  </si>
+  <si>
+    <t>GO:0006418</t>
+  </si>
+  <si>
+    <t>GO:0006506</t>
+  </si>
+  <si>
+    <t>GO:0006801</t>
+  </si>
+  <si>
+    <t>GO:0007271</t>
+  </si>
+  <si>
+    <t>GO:0007346</t>
+  </si>
+  <si>
+    <t>GO:0007398</t>
+  </si>
+  <si>
+    <t>gorilla,orangutan,monkey</t>
+  </si>
+  <si>
+    <t>GO:0010971</t>
+  </si>
+  <si>
+    <t>GO:0019843</t>
+  </si>
+  <si>
+    <t>chimp,gorilla,orangutan</t>
+  </si>
+  <si>
+    <t>GO:0030134</t>
+  </si>
+  <si>
+    <t>GO:0030667</t>
+  </si>
+  <si>
+    <t>GO:0030904</t>
+  </si>
+  <si>
+    <t>GO:0031624</t>
+  </si>
+  <si>
+    <t>GO:0031641</t>
+  </si>
+  <si>
+    <t>chimp,orangutan,monkey</t>
+  </si>
+  <si>
+    <t>GO:0042326</t>
+  </si>
+  <si>
+    <t>GO:0043393</t>
+  </si>
+  <si>
+    <t>GO:0043425</t>
+  </si>
+  <si>
+    <t>GO:0043984</t>
+  </si>
+  <si>
+    <t>GO:0047496</t>
+  </si>
+  <si>
+    <t>GO:0060317</t>
+  </si>
+  <si>
+    <t>GO:0060412</t>
+  </si>
+  <si>
+    <t>GO:0070016</t>
+  </si>
+  <si>
+    <t>GO:0072332</t>
+  </si>
+  <si>
+    <t>GO:0000118</t>
+  </si>
+  <si>
+    <t>GO:0005545</t>
+  </si>
+  <si>
+    <t>GO:0006362</t>
+  </si>
+  <si>
+    <t>GO:0006368</t>
+  </si>
+  <si>
+    <t>GO:0007259</t>
+  </si>
+  <si>
+    <t>GO:0009416</t>
+  </si>
+  <si>
+    <t>GO:0012507</t>
+  </si>
+  <si>
+    <t>GO:0014003</t>
+  </si>
+  <si>
+    <t>GO:0014823</t>
+  </si>
+  <si>
+    <t>GO:0030155</t>
+  </si>
+  <si>
+    <t>GO:0035666</t>
+  </si>
+  <si>
+    <t>chimp,gorilla,monkey</t>
+  </si>
+  <si>
+    <t>GO:0040008</t>
+  </si>
+  <si>
+    <t>GO:0042692</t>
+  </si>
+  <si>
+    <t>GO:0043523</t>
+  </si>
+  <si>
+    <t>GO:0044297</t>
+  </si>
+  <si>
+    <t>GO:0045445</t>
+  </si>
+  <si>
+    <t>GO:1903506</t>
+  </si>
+  <si>
+    <t>GO:2000378</t>
+  </si>
+  <si>
+    <t>GO:0000982</t>
+  </si>
+  <si>
+    <t>GO:0004623</t>
+  </si>
+  <si>
+    <t>GO:0005319</t>
+  </si>
+  <si>
+    <t>GO:0006298</t>
+  </si>
+  <si>
+    <t>GO:0007339</t>
+  </si>
+  <si>
+    <t>GO:0008009</t>
+  </si>
+  <si>
+    <t>GO:0015721</t>
+  </si>
+  <si>
+    <t>GO:0032781</t>
+  </si>
+  <si>
+    <t>GO:0045717</t>
+  </si>
+  <si>
+    <t>GO:0045931</t>
+  </si>
+  <si>
+    <t>GO:0051000</t>
+  </si>
+  <si>
+    <t>GO:0070402</t>
+  </si>
+  <si>
+    <t>GO:0071353</t>
+  </si>
+  <si>
+    <t>GO:0071363</t>
+  </si>
+  <si>
+    <t>GO:1903959</t>
+  </si>
+  <si>
+    <t>GO:0000421</t>
+  </si>
+  <si>
+    <t>GO:0002028</t>
+  </si>
+  <si>
+    <t>GO:0006958</t>
+  </si>
+  <si>
+    <t>GO:0031402</t>
+  </si>
+  <si>
+    <t>GO:0032793</t>
+  </si>
+  <si>
+    <t>GO:0035902</t>
+  </si>
+  <si>
+    <t>GO:0043198</t>
+  </si>
+  <si>
+    <t>GO:0050434</t>
+  </si>
+  <si>
+    <t>GO:0051895</t>
+  </si>
+  <si>
+    <t>GO:0055072</t>
+  </si>
+  <si>
+    <t>GO:0097193</t>
+  </si>
+  <si>
+    <t>GO:0000159</t>
+  </si>
+  <si>
+    <t>GO:0000185</t>
+  </si>
+  <si>
+    <t>GO:0001895</t>
+  </si>
+  <si>
+    <t>GO:0004683</t>
+  </si>
+  <si>
+    <t>GO:0004857</t>
+  </si>
+  <si>
+    <t>GO:0004864</t>
+  </si>
+  <si>
+    <t>GO:0005778</t>
+  </si>
+  <si>
+    <t>GO:0006171</t>
+  </si>
+  <si>
+    <t>GO:0006294</t>
+  </si>
+  <si>
+    <t>GO:0007193</t>
+  </si>
+  <si>
+    <t>GO:0008135</t>
+  </si>
+  <si>
+    <t>GO:0008654</t>
+  </si>
+  <si>
+    <t>GO:0009617</t>
+  </si>
+  <si>
+    <t>GO:0017148</t>
+  </si>
+  <si>
+    <t>GO:0030897</t>
+  </si>
+  <si>
+    <t>GO:0032947</t>
+  </si>
+  <si>
+    <t>GO:003327</t>
+  </si>
+  <si>
+    <t>GO:0042476</t>
+  </si>
+  <si>
+    <t>GO:0045742</t>
+  </si>
+  <si>
+    <t>GO:0051497</t>
+  </si>
+  <si>
+    <t>GO:0070064</t>
+  </si>
+  <si>
+    <t>GO:0070584</t>
+  </si>
+  <si>
+    <t>GO:0070987</t>
+  </si>
+  <si>
+    <t>GO:0001104</t>
+  </si>
+  <si>
+    <t>GO:0001892</t>
+  </si>
+  <si>
+    <t>GO:0003712</t>
+  </si>
+  <si>
+    <t>GO:0004722</t>
+  </si>
+  <si>
+    <t>GO:0005669</t>
+  </si>
+  <si>
+    <t>GO:0005798</t>
+  </si>
+  <si>
+    <t>GO:0006297</t>
+  </si>
+  <si>
+    <t>GO:0006488</t>
+  </si>
+  <si>
+    <t>GO:0006511</t>
+  </si>
+  <si>
+    <t>GO:0009952</t>
+  </si>
+  <si>
+    <t>GO:0017025</t>
+  </si>
+  <si>
+    <t>GO:0019915</t>
+  </si>
+  <si>
+    <t>GO:0030148</t>
+  </si>
+  <si>
+    <t>GO:0030215</t>
+  </si>
+  <si>
+    <t>GO:0031418</t>
+  </si>
+  <si>
+    <t>GO:0034198</t>
+  </si>
+  <si>
+    <t>GO:0034512</t>
+  </si>
+  <si>
+    <t>GO:0036152</t>
+  </si>
+  <si>
+    <t>GO:0043011</t>
+  </si>
+  <si>
+    <t>GO:0043560</t>
+  </si>
+  <si>
+    <t>GO:0048514</t>
+  </si>
+  <si>
+    <t>GO:2000785</t>
+  </si>
+  <si>
+    <t>GO:0000717</t>
+  </si>
+  <si>
+    <t>GO:0001541</t>
+  </si>
+  <si>
+    <t>GO:0001569</t>
+  </si>
+  <si>
+    <t>GO:0001819</t>
+  </si>
+  <si>
+    <t>GO:0003823</t>
+  </si>
+  <si>
+    <t>GO:0004812</t>
+  </si>
+  <si>
+    <t>GO:0005681</t>
+  </si>
+  <si>
+    <t>GO:0006296</t>
+  </si>
+  <si>
+    <t>GO:0006261</t>
+  </si>
+  <si>
+    <t>GO:0006928</t>
+  </si>
+  <si>
+    <t>GO:0017048</t>
+  </si>
+  <si>
+    <t>GO:0030057</t>
+  </si>
+  <si>
+    <t>GO:0031011</t>
+  </si>
+  <si>
+    <t>GO:0031267</t>
+  </si>
+  <si>
+    <t>GO:0035024</t>
+  </si>
+  <si>
+    <t>GO:0035994</t>
+  </si>
+  <si>
+    <t>GO:0043014</t>
+  </si>
+  <si>
+    <t>GO:0043484</t>
+  </si>
+  <si>
+    <t>GO:0046716</t>
+  </si>
+  <si>
+    <t>GO:0048025</t>
+  </si>
+  <si>
+    <t>GO:0050681</t>
+  </si>
+  <si>
+    <t>GO:0055093</t>
+  </si>
+  <si>
+    <t>GO:0090023</t>
+  </si>
+  <si>
+    <t>GO:0090398</t>
+  </si>
+  <si>
+    <t>GO:1900087</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -459,13 +938,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -797,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1710,6 +2201,2571 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148:C181"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>180</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" t="s">
+        <v>40</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>40</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>192</v>
+      </c>
+      <c r="B59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>42</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>197</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>42</v>
+      </c>
+      <c r="E64" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>198</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>199</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>42</v>
+      </c>
+      <c r="E68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>201</v>
+      </c>
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E69" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>42</v>
+      </c>
+      <c r="E70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>167</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" t="s">
+        <v>42</v>
+      </c>
+      <c r="E71" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>202</v>
+      </c>
+      <c r="B72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" t="s">
+        <v>42</v>
+      </c>
+      <c r="E73" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>204</v>
+      </c>
+      <c r="B74" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75" t="s">
+        <v>31</v>
+      </c>
+      <c r="C75" t="s">
+        <v>42</v>
+      </c>
+      <c r="E75" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>206</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>42</v>
+      </c>
+      <c r="E76" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>207</v>
+      </c>
+      <c r="B77" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" t="s">
+        <v>42</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>208</v>
+      </c>
+      <c r="B78" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" t="s">
+        <v>42</v>
+      </c>
+      <c r="E78" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" t="s">
+        <v>37</v>
+      </c>
+      <c r="C79" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>210</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E80" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>211</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" t="s">
+        <v>37</v>
+      </c>
+      <c r="C82" t="s">
+        <v>45</v>
+      </c>
+      <c r="E82" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>45</v>
+      </c>
+      <c r="E83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>212</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>213</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>45</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" t="s">
+        <v>45</v>
+      </c>
+      <c r="E86" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>45</v>
+      </c>
+      <c r="E87" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>54</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>45</v>
+      </c>
+      <c r="E88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>45</v>
+      </c>
+      <c r="E89" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>217</v>
+      </c>
+      <c r="B90" t="s">
+        <v>31</v>
+      </c>
+      <c r="C90" t="s">
+        <v>45</v>
+      </c>
+      <c r="E90" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>218</v>
+      </c>
+      <c r="B91" t="s">
+        <v>27</v>
+      </c>
+      <c r="C91" t="s">
+        <v>45</v>
+      </c>
+      <c r="E91" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>219</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>45</v>
+      </c>
+      <c r="E92" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>220</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" t="s">
+        <v>58</v>
+      </c>
+      <c r="E93" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>221</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>58</v>
+      </c>
+      <c r="E94" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>209</v>
+      </c>
+      <c r="B95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" t="s">
+        <v>58</v>
+      </c>
+      <c r="E95" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>222</v>
+      </c>
+      <c r="B96" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" t="s">
+        <v>58</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>223</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" t="s">
+        <v>58</v>
+      </c>
+      <c r="E97" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>224</v>
+      </c>
+      <c r="B98" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" t="s">
+        <v>58</v>
+      </c>
+      <c r="E98" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>225</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>58</v>
+      </c>
+      <c r="E99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>226</v>
+      </c>
+      <c r="B100" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" t="s">
+        <v>58</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>227</v>
+      </c>
+      <c r="B101" t="s">
+        <v>37</v>
+      </c>
+      <c r="C101" t="s">
+        <v>58</v>
+      </c>
+      <c r="E101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>228</v>
+      </c>
+      <c r="B102" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102" t="s">
+        <v>58</v>
+      </c>
+      <c r="E102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>229</v>
+      </c>
+      <c r="B103" t="s">
+        <v>27</v>
+      </c>
+      <c r="C103" t="s">
+        <v>58</v>
+      </c>
+      <c r="E103" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>230</v>
+      </c>
+      <c r="B104" t="s">
+        <v>4</v>
+      </c>
+      <c r="C104" t="s">
+        <v>58</v>
+      </c>
+      <c r="E104" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>231</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" t="s">
+        <v>58</v>
+      </c>
+      <c r="E105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>232</v>
+      </c>
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106" t="s">
+        <v>58</v>
+      </c>
+      <c r="E106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>233</v>
+      </c>
+      <c r="B107" t="s">
+        <v>27</v>
+      </c>
+      <c r="C107" t="s">
+        <v>58</v>
+      </c>
+      <c r="E107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>39</v>
+      </c>
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" t="s">
+        <v>58</v>
+      </c>
+      <c r="E108" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>234</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>58</v>
+      </c>
+      <c r="E109" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>235</v>
+      </c>
+      <c r="B110" t="s">
+        <v>27</v>
+      </c>
+      <c r="C110" t="s">
+        <v>58</v>
+      </c>
+      <c r="E110" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>236</v>
+      </c>
+      <c r="B111" t="s">
+        <v>37</v>
+      </c>
+      <c r="C111" t="s">
+        <v>58</v>
+      </c>
+      <c r="E111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>237</v>
+      </c>
+      <c r="B112" t="s">
+        <v>71</v>
+      </c>
+      <c r="C112" t="s">
+        <v>58</v>
+      </c>
+      <c r="E112" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>238</v>
+      </c>
+      <c r="B113" t="s">
+        <v>27</v>
+      </c>
+      <c r="C113" t="s">
+        <v>58</v>
+      </c>
+      <c r="E113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>170</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+      <c r="C114" t="s">
+        <v>58</v>
+      </c>
+      <c r="E114" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>239</v>
+      </c>
+      <c r="B115" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" t="s">
+        <v>58</v>
+      </c>
+      <c r="E115" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>147</v>
+      </c>
+      <c r="B116" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" t="s">
+        <v>58</v>
+      </c>
+      <c r="E116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>240</v>
+      </c>
+      <c r="B117" t="s">
+        <v>37</v>
+      </c>
+      <c r="C117" t="s">
+        <v>58</v>
+      </c>
+      <c r="E117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>241</v>
+      </c>
+      <c r="B118" t="s">
+        <v>37</v>
+      </c>
+      <c r="C118" t="s">
+        <v>58</v>
+      </c>
+      <c r="E118" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>242</v>
+      </c>
+      <c r="B119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119" t="s">
+        <v>58</v>
+      </c>
+      <c r="E119" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>243</v>
+      </c>
+      <c r="B120" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" t="s">
+        <v>67</v>
+      </c>
+      <c r="E120" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>244</v>
+      </c>
+      <c r="B121" t="s">
+        <v>31</v>
+      </c>
+      <c r="C121" t="s">
+        <v>67</v>
+      </c>
+      <c r="E121" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>245</v>
+      </c>
+      <c r="B122" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122" t="s">
+        <v>67</v>
+      </c>
+      <c r="E122" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>246</v>
+      </c>
+      <c r="B123" t="s">
+        <v>31</v>
+      </c>
+      <c r="C123" t="s">
+        <v>67</v>
+      </c>
+      <c r="E123" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" t="s">
+        <v>67</v>
+      </c>
+      <c r="E124" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>247</v>
+      </c>
+      <c r="B125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" t="s">
+        <v>67</v>
+      </c>
+      <c r="E125" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" t="s">
+        <v>67</v>
+      </c>
+      <c r="E126" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>249</v>
+      </c>
+      <c r="B127" t="s">
+        <v>27</v>
+      </c>
+      <c r="C127" t="s">
+        <v>67</v>
+      </c>
+      <c r="E127" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>178</v>
+      </c>
+      <c r="B128" t="s">
+        <v>31</v>
+      </c>
+      <c r="C128" t="s">
+        <v>67</v>
+      </c>
+      <c r="E128" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>250</v>
+      </c>
+      <c r="B129" t="s">
+        <v>31</v>
+      </c>
+      <c r="C129" t="s">
+        <v>67</v>
+      </c>
+      <c r="E129" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>251</v>
+      </c>
+      <c r="B130" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" t="s">
+        <v>67</v>
+      </c>
+      <c r="E130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>252</v>
+      </c>
+      <c r="B131" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" t="s">
+        <v>67</v>
+      </c>
+      <c r="E131" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>253</v>
+      </c>
+      <c r="B132" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" t="s">
+        <v>67</v>
+      </c>
+      <c r="E132" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>254</v>
+      </c>
+      <c r="B133" t="s">
+        <v>31</v>
+      </c>
+      <c r="C133" t="s">
+        <v>67</v>
+      </c>
+      <c r="E133" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>255</v>
+      </c>
+      <c r="B134" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" t="s">
+        <v>67</v>
+      </c>
+      <c r="E134" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>256</v>
+      </c>
+      <c r="B135" t="s">
+        <v>11</v>
+      </c>
+      <c r="C135" t="s">
+        <v>67</v>
+      </c>
+      <c r="E135" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>257</v>
+      </c>
+      <c r="B136" t="s">
+        <v>11</v>
+      </c>
+      <c r="C136" t="s">
+        <v>67</v>
+      </c>
+      <c r="E136" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>258</v>
+      </c>
+      <c r="B137" t="s">
+        <v>27</v>
+      </c>
+      <c r="C137" t="s">
+        <v>67</v>
+      </c>
+      <c r="E137" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>259</v>
+      </c>
+      <c r="B138" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138" t="s">
+        <v>67</v>
+      </c>
+      <c r="E138" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>185</v>
+      </c>
+      <c r="B139" t="s">
+        <v>27</v>
+      </c>
+      <c r="C139" t="s">
+        <v>67</v>
+      </c>
+      <c r="E139" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>260</v>
+      </c>
+      <c r="B140" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140" t="s">
+        <v>67</v>
+      </c>
+      <c r="E140" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>261</v>
+      </c>
+      <c r="B141" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" t="s">
+        <v>67</v>
+      </c>
+      <c r="E141" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>262</v>
+      </c>
+      <c r="B142" t="s">
+        <v>31</v>
+      </c>
+      <c r="C142" t="s">
+        <v>67</v>
+      </c>
+      <c r="E142" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>263</v>
+      </c>
+      <c r="B143" t="s">
+        <v>31</v>
+      </c>
+      <c r="C143" t="s">
+        <v>67</v>
+      </c>
+      <c r="E143" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>69</v>
+      </c>
+      <c r="B144" t="s">
+        <v>37</v>
+      </c>
+      <c r="C144" t="s">
+        <v>67</v>
+      </c>
+      <c r="E144" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>219</v>
+      </c>
+      <c r="B145" t="s">
+        <v>27</v>
+      </c>
+      <c r="C145" t="s">
+        <v>67</v>
+      </c>
+      <c r="E145" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>192</v>
+      </c>
+      <c r="B146" t="s">
+        <v>31</v>
+      </c>
+      <c r="C146" t="s">
+        <v>67</v>
+      </c>
+      <c r="E146" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>264</v>
+      </c>
+      <c r="B147" t="s">
+        <v>31</v>
+      </c>
+      <c r="C147" t="s">
+        <v>67</v>
+      </c>
+      <c r="E147" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>70</v>
+      </c>
+      <c r="B148" t="s">
+        <v>71</v>
+      </c>
+      <c r="C148" t="s">
+        <v>72</v>
+      </c>
+      <c r="E148" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>265</v>
+      </c>
+      <c r="B149" t="s">
+        <v>31</v>
+      </c>
+      <c r="C149" t="s">
+        <v>72</v>
+      </c>
+      <c r="E149" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>266</v>
+      </c>
+      <c r="B150" t="s">
+        <v>37</v>
+      </c>
+      <c r="C150" t="s">
+        <v>72</v>
+      </c>
+      <c r="E150" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>267</v>
+      </c>
+      <c r="B151" t="s">
+        <v>31</v>
+      </c>
+      <c r="C151" t="s">
+        <v>72</v>
+      </c>
+      <c r="E151" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>268</v>
+      </c>
+      <c r="B152" t="s">
+        <v>37</v>
+      </c>
+      <c r="C152" t="s">
+        <v>72</v>
+      </c>
+      <c r="E152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>269</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" t="s">
+        <v>72</v>
+      </c>
+      <c r="E153" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>270</v>
+      </c>
+      <c r="B154" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" t="s">
+        <v>72</v>
+      </c>
+      <c r="E154" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>271</v>
+      </c>
+      <c r="B155" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155" t="s">
+        <v>72</v>
+      </c>
+      <c r="E155" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>228</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
+      <c r="C156" t="s">
+        <v>72</v>
+      </c>
+      <c r="E156" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>272</v>
+      </c>
+      <c r="B157" t="s">
+        <v>31</v>
+      </c>
+      <c r="C157" t="s">
+        <v>72</v>
+      </c>
+      <c r="E157" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>273</v>
+      </c>
+      <c r="B158" t="s">
+        <v>31</v>
+      </c>
+      <c r="C158" t="s">
+        <v>72</v>
+      </c>
+      <c r="E158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>152</v>
+      </c>
+      <c r="B159" t="s">
+        <v>37</v>
+      </c>
+      <c r="C159" t="s">
+        <v>72</v>
+      </c>
+      <c r="E159" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>274</v>
+      </c>
+      <c r="B160" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" t="s">
+        <v>72</v>
+      </c>
+      <c r="E160" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>75</v>
+      </c>
+      <c r="B161" t="s">
+        <v>71</v>
+      </c>
+      <c r="C161" t="s">
+        <v>72</v>
+      </c>
+      <c r="E161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>275</v>
+      </c>
+      <c r="B162" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" t="s">
+        <v>72</v>
+      </c>
+      <c r="E162" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>276</v>
+      </c>
+      <c r="B163" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" t="s">
+        <v>72</v>
+      </c>
+      <c r="E163" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>277</v>
+      </c>
+      <c r="B164" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" t="s">
+        <v>72</v>
+      </c>
+      <c r="E164" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>278</v>
+      </c>
+      <c r="B165" t="s">
+        <v>27</v>
+      </c>
+      <c r="C165" t="s">
+        <v>72</v>
+      </c>
+      <c r="E165" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>80</v>
+      </c>
+      <c r="B166" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" t="s">
+        <v>72</v>
+      </c>
+      <c r="E166" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>279</v>
+      </c>
+      <c r="B167" t="s">
+        <v>4</v>
+      </c>
+      <c r="C167" t="s">
+        <v>72</v>
+      </c>
+      <c r="E167" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>280</v>
+      </c>
+      <c r="B168" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168" t="s">
+        <v>72</v>
+      </c>
+      <c r="E168" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>281</v>
+      </c>
+      <c r="B169" t="s">
+        <v>4</v>
+      </c>
+      <c r="C169" t="s">
+        <v>72</v>
+      </c>
+      <c r="E169" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>282</v>
+      </c>
+      <c r="B170" t="s">
+        <v>4</v>
+      </c>
+      <c r="C170" t="s">
+        <v>72</v>
+      </c>
+      <c r="E170" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>82</v>
+      </c>
+      <c r="B171" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" t="s">
+        <v>72</v>
+      </c>
+      <c r="E171" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>283</v>
+      </c>
+      <c r="B172" t="s">
+        <v>37</v>
+      </c>
+      <c r="C172" t="s">
+        <v>72</v>
+      </c>
+      <c r="E172" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>284</v>
+      </c>
+      <c r="B173" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173" t="s">
+        <v>72</v>
+      </c>
+      <c r="E173" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>285</v>
+      </c>
+      <c r="B174" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174" t="s">
+        <v>72</v>
+      </c>
+      <c r="E174" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>286</v>
+      </c>
+      <c r="B175" t="s">
+        <v>71</v>
+      </c>
+      <c r="C175" t="s">
+        <v>72</v>
+      </c>
+      <c r="E175" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>172</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4</v>
+      </c>
+      <c r="C176" t="s">
+        <v>72</v>
+      </c>
+      <c r="E176" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>207</v>
+      </c>
+      <c r="B177" t="s">
+        <v>37</v>
+      </c>
+      <c r="C177" t="s">
+        <v>72</v>
+      </c>
+      <c r="E177" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>287</v>
+      </c>
+      <c r="B178" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178" t="s">
+        <v>72</v>
+      </c>
+      <c r="E178" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>288</v>
+      </c>
+      <c r="B179" t="s">
+        <v>4</v>
+      </c>
+      <c r="C179" t="s">
+        <v>72</v>
+      </c>
+      <c r="E179" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>219</v>
+      </c>
+      <c r="B180" t="s">
+        <v>27</v>
+      </c>
+      <c r="C180" t="s">
+        <v>72</v>
+      </c>
+      <c r="E180" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>289</v>
+      </c>
+      <c r="B181" t="s">
+        <v>71</v>
+      </c>
+      <c r="C181" t="s">
+        <v>72</v>
+      </c>
+      <c r="E181" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
bioperl code to extract bed file elements
</commit_message>
<xml_diff>
--- a/sigGOterms.xlsx
+++ b/sigGOterms.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1020" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="First ver." sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="303">
   <si>
     <t>organ</t>
   </si>
@@ -887,6 +887,48 @@
   </si>
   <si>
     <t>GO:0034612</t>
+  </si>
+  <si>
+    <t>transcription factor TFTC complex</t>
+  </si>
+  <si>
+    <t>tRNA aminoacylation for protein translation</t>
+  </si>
+  <si>
+    <t>ER to Golgi vesicle</t>
+  </si>
+  <si>
+    <t>negative regulation of phosphorylation</t>
+  </si>
+  <si>
+    <t>armadillo repeat domain binding</t>
+  </si>
+  <si>
+    <t>histone deacetylation complex</t>
+  </si>
+  <si>
+    <t>jak-stat cascade</t>
+  </si>
+  <si>
+    <t>response to bacterium</t>
+  </si>
+  <si>
+    <t>vesicle transport along microtuble</t>
+  </si>
+  <si>
+    <t>protein serine/theonine phosphotase activity</t>
+  </si>
+  <si>
+    <t>desmosome</t>
+  </si>
+  <si>
+    <t>small-subunit processome</t>
+  </si>
+  <si>
+    <t>alpha tubulin binding</t>
+  </si>
+  <si>
+    <t>sig</t>
   </si>
 </sst>
 </file>
@@ -2209,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H173" sqref="H173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2224,7 +2266,7 @@
     <col min="5" max="5" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -2240,8 +2282,11 @@
       <c r="E1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -2254,8 +2299,12 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <f t="shared" ref="F2:F5" si="0">IF(D2&lt;&gt;"",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -2268,8 +2317,12 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -2282,8 +2335,12 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -2296,8 +2353,12 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2307,11 +2368,18 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6" t="s">
+        <v>289</v>
+      </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <f>IF(D6&lt;&gt;"",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -2324,8 +2392,12 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <f t="shared" ref="F7:F70" si="1">IF(D7&lt;&gt;"",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -2338,8 +2410,12 @@
       <c r="E8" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -2352,8 +2428,12 @@
       <c r="E9" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -2366,8 +2446,12 @@
       <c r="E10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>146</v>
       </c>
@@ -2380,8 +2464,12 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>147</v>
       </c>
@@ -2394,8 +2482,12 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>148</v>
       </c>
@@ -2408,8 +2500,12 @@
       <c r="E13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -2422,8 +2518,12 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -2433,11 +2533,18 @@
       <c r="C15" t="s">
         <v>28</v>
       </c>
+      <c r="D15" t="s">
+        <v>290</v>
+      </c>
       <c r="E15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>151</v>
       </c>
@@ -2450,8 +2557,12 @@
       <c r="E16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -2464,8 +2575,12 @@
       <c r="E17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>137</v>
       </c>
@@ -2478,8 +2593,12 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -2492,8 +2611,12 @@
       <c r="E19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -2506,8 +2629,12 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -2520,8 +2647,12 @@
       <c r="E21" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>157</v>
       </c>
@@ -2534,8 +2665,12 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>158</v>
       </c>
@@ -2548,8 +2683,12 @@
       <c r="E23" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -2562,8 +2701,12 @@
       <c r="E24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>160</v>
       </c>
@@ -2573,11 +2716,18 @@
       <c r="C25" t="s">
         <v>28</v>
       </c>
+      <c r="D25" t="s">
+        <v>291</v>
+      </c>
       <c r="E25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -2590,8 +2740,12 @@
       <c r="E26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2604,8 +2758,12 @@
       <c r="E27" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>161</v>
       </c>
@@ -2618,8 +2776,12 @@
       <c r="E28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>162</v>
       </c>
@@ -2632,8 +2794,12 @@
       <c r="E29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>163</v>
       </c>
@@ -2646,8 +2812,12 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>164</v>
       </c>
@@ -2660,8 +2830,12 @@
       <c r="E31" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>166</v>
       </c>
@@ -2671,11 +2845,18 @@
       <c r="C32" t="s">
         <v>28</v>
       </c>
+      <c r="D32" t="s">
+        <v>292</v>
+      </c>
       <c r="E32" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>167</v>
       </c>
@@ -2688,8 +2869,12 @@
       <c r="E33" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>168</v>
       </c>
@@ -2702,8 +2887,12 @@
       <c r="E34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -2716,8 +2905,12 @@
       <c r="E35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>170</v>
       </c>
@@ -2730,8 +2923,12 @@
       <c r="E36" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>171</v>
       </c>
@@ -2744,8 +2941,12 @@
       <c r="E37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -2758,8 +2959,12 @@
       <c r="E38" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>173</v>
       </c>
@@ -2769,11 +2974,18 @@
       <c r="C39" t="s">
         <v>28</v>
       </c>
+      <c r="D39" t="s">
+        <v>293</v>
+      </c>
       <c r="E39" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -2786,8 +2998,12 @@
       <c r="E40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2800,8 +3016,12 @@
       <c r="E41" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -2811,11 +3031,18 @@
       <c r="C42" t="s">
         <v>40</v>
       </c>
+      <c r="D42" t="s">
+        <v>294</v>
+      </c>
       <c r="E42" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>176</v>
       </c>
@@ -2828,8 +3055,12 @@
       <c r="E43" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>177</v>
       </c>
@@ -2842,8 +3073,12 @@
       <c r="E44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>178</v>
       </c>
@@ -2856,8 +3091,12 @@
       <c r="E45" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>179</v>
       </c>
@@ -2867,11 +3106,18 @@
       <c r="C46" t="s">
         <v>40</v>
       </c>
+      <c r="D46" t="s">
+        <v>295</v>
+      </c>
       <c r="E46" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>180</v>
       </c>
@@ -2884,8 +3130,12 @@
       <c r="E47" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>181</v>
       </c>
@@ -2898,8 +3148,12 @@
       <c r="E48" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>182</v>
       </c>
@@ -2912,8 +3166,12 @@
       <c r="E49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -2926,8 +3184,12 @@
       <c r="E50" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -2940,8 +3202,12 @@
       <c r="E51" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>184</v>
       </c>
@@ -2954,8 +3220,12 @@
       <c r="E52" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>185</v>
       </c>
@@ -2968,8 +3238,12 @@
       <c r="E53" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>187</v>
       </c>
@@ -2982,8 +3256,12 @@
       <c r="E54" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>188</v>
       </c>
@@ -2996,8 +3274,12 @@
       <c r="E55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>189</v>
       </c>
@@ -3010,8 +3292,12 @@
       <c r="E56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>190</v>
       </c>
@@ -3024,8 +3310,12 @@
       <c r="E57" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>191</v>
       </c>
@@ -3038,8 +3328,12 @@
       <c r="E58" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>192</v>
       </c>
@@ -3052,8 +3346,12 @@
       <c r="E59" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>193</v>
       </c>
@@ -3066,8 +3364,12 @@
       <c r="E60" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>194</v>
       </c>
@@ -3080,8 +3382,12 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>195</v>
       </c>
@@ -3094,8 +3400,12 @@
       <c r="E62" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>196</v>
       </c>
@@ -3108,8 +3418,12 @@
       <c r="E63" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>197</v>
       </c>
@@ -3122,8 +3436,12 @@
       <c r="E64" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>198</v>
       </c>
@@ -3136,8 +3454,12 @@
       <c r="E65" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -3150,8 +3472,12 @@
       <c r="E66" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>200</v>
       </c>
@@ -3164,8 +3490,12 @@
       <c r="E67" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -3178,8 +3508,12 @@
       <c r="E68" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -3192,8 +3526,12 @@
       <c r="E69" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -3206,8 +3544,12 @@
       <c r="E70" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>167</v>
       </c>
@@ -3220,8 +3562,12 @@
       <c r="E71" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71">
+        <f t="shared" ref="F71:F134" si="2">IF(D71&lt;&gt;"",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>202</v>
       </c>
@@ -3234,8 +3580,12 @@
       <c r="E72" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>203</v>
       </c>
@@ -3248,8 +3598,12 @@
       <c r="E73" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>204</v>
       </c>
@@ -3262,8 +3616,12 @@
       <c r="E74" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>205</v>
       </c>
@@ -3276,8 +3634,12 @@
       <c r="E75" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>206</v>
       </c>
@@ -3290,8 +3652,12 @@
       <c r="E76" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>207</v>
       </c>
@@ -3304,8 +3670,12 @@
       <c r="E77" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>208</v>
       </c>
@@ -3318,8 +3688,12 @@
       <c r="E78" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>209</v>
       </c>
@@ -3332,8 +3706,12 @@
       <c r="E79" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>210</v>
       </c>
@@ -3346,8 +3724,12 @@
       <c r="E80" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>211</v>
       </c>
@@ -3360,8 +3742,12 @@
       <c r="E81" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -3374,8 +3760,12 @@
       <c r="E82" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>39</v>
       </c>
@@ -3388,8 +3778,12 @@
       <c r="E83" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>212</v>
       </c>
@@ -3402,8 +3796,12 @@
       <c r="E84" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>213</v>
       </c>
@@ -3416,8 +3814,12 @@
       <c r="E85" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>214</v>
       </c>
@@ -3430,8 +3832,12 @@
       <c r="E86" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -3444,8 +3850,12 @@
       <c r="E87" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>54</v>
       </c>
@@ -3458,8 +3868,12 @@
       <c r="E88" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>216</v>
       </c>
@@ -3472,8 +3886,12 @@
       <c r="E89" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>217</v>
       </c>
@@ -3486,8 +3904,12 @@
       <c r="E90" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>218</v>
       </c>
@@ -3500,8 +3922,12 @@
       <c r="E91" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>219</v>
       </c>
@@ -3514,8 +3940,12 @@
       <c r="E92" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>220</v>
       </c>
@@ -3528,8 +3958,12 @@
       <c r="E93" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>221</v>
       </c>
@@ -3542,8 +3976,12 @@
       <c r="E94" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>209</v>
       </c>
@@ -3556,8 +3994,12 @@
       <c r="E95" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>222</v>
       </c>
@@ -3570,8 +4012,12 @@
       <c r="E96" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>223</v>
       </c>
@@ -3584,8 +4030,12 @@
       <c r="E97" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>224</v>
       </c>
@@ -3598,8 +4048,12 @@
       <c r="E98" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>225</v>
       </c>
@@ -3612,8 +4066,12 @@
       <c r="E99" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>226</v>
       </c>
@@ -3626,8 +4084,12 @@
       <c r="E100" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>227</v>
       </c>
@@ -3640,8 +4102,12 @@
       <c r="E101" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>228</v>
       </c>
@@ -3654,8 +4120,12 @@
       <c r="E102" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>229</v>
       </c>
@@ -3668,8 +4138,12 @@
       <c r="E103" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>230</v>
       </c>
@@ -3682,8 +4156,12 @@
       <c r="E104" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>231</v>
       </c>
@@ -3696,8 +4174,12 @@
       <c r="E105" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>232</v>
       </c>
@@ -3707,11 +4189,18 @@
       <c r="C106" t="s">
         <v>58</v>
       </c>
+      <c r="D106" t="s">
+        <v>296</v>
+      </c>
       <c r="E106" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>233</v>
       </c>
@@ -3724,8 +4213,12 @@
       <c r="E107" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>39</v>
       </c>
@@ -3738,8 +4231,12 @@
       <c r="E108" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>234</v>
       </c>
@@ -3752,8 +4249,12 @@
       <c r="E109" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>235</v>
       </c>
@@ -3766,8 +4267,12 @@
       <c r="E110" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>62</v>
       </c>
@@ -3780,8 +4285,12 @@
       <c r="E111" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>236</v>
       </c>
@@ -3794,8 +4303,12 @@
       <c r="E112" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>237</v>
       </c>
@@ -3808,8 +4321,12 @@
       <c r="E113" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>170</v>
       </c>
@@ -3819,11 +4336,18 @@
       <c r="C114" t="s">
         <v>58</v>
       </c>
+      <c r="D114" t="s">
+        <v>297</v>
+      </c>
       <c r="E114" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>238</v>
       </c>
@@ -3836,8 +4360,12 @@
       <c r="E115" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>147</v>
       </c>
@@ -3850,8 +4378,12 @@
       <c r="E116" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>239</v>
       </c>
@@ -3864,8 +4396,12 @@
       <c r="E117" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>240</v>
       </c>
@@ -3878,8 +4414,12 @@
       <c r="E118" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>241</v>
       </c>
@@ -3892,8 +4432,12 @@
       <c r="E119" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>242</v>
       </c>
@@ -3906,8 +4450,12 @@
       <c r="E120" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>243</v>
       </c>
@@ -3920,8 +4468,12 @@
       <c r="E121" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>244</v>
       </c>
@@ -3934,8 +4486,12 @@
       <c r="E122" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>245</v>
       </c>
@@ -3945,11 +4501,18 @@
       <c r="C123" t="s">
         <v>67</v>
       </c>
+      <c r="D123" t="s">
+        <v>298</v>
+      </c>
       <c r="E123" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>12</v>
       </c>
@@ -3962,8 +4525,12 @@
       <c r="E124" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>246</v>
       </c>
@@ -3976,8 +4543,12 @@
       <c r="E125" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>247</v>
       </c>
@@ -3990,8 +4561,12 @@
       <c r="E126" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>248</v>
       </c>
@@ -4004,8 +4579,12 @@
       <c r="E127" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>178</v>
       </c>
@@ -4018,8 +4597,12 @@
       <c r="E128" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>249</v>
       </c>
@@ -4032,8 +4615,12 @@
       <c r="E129" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>250</v>
       </c>
@@ -4046,8 +4633,12 @@
       <c r="E130" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>251</v>
       </c>
@@ -4060,8 +4651,12 @@
       <c r="E131" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>252</v>
       </c>
@@ -4074,8 +4669,12 @@
       <c r="E132" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>253</v>
       </c>
@@ -4088,8 +4687,12 @@
       <c r="E133" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>254</v>
       </c>
@@ -4102,8 +4705,12 @@
       <c r="E134" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>255</v>
       </c>
@@ -4116,8 +4723,12 @@
       <c r="E135" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135">
+        <f t="shared" ref="F135:F181" si="3">IF(D135&lt;&gt;"",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>256</v>
       </c>
@@ -4130,8 +4741,12 @@
       <c r="E136" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>257</v>
       </c>
@@ -4144,8 +4759,12 @@
       <c r="E137" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>288</v>
       </c>
@@ -4158,8 +4777,12 @@
       <c r="E138" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>185</v>
       </c>
@@ -4172,8 +4795,12 @@
       <c r="E139" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>258</v>
       </c>
@@ -4186,8 +4813,12 @@
       <c r="E140" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>259</v>
       </c>
@@ -4200,8 +4831,12 @@
       <c r="E141" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>260</v>
       </c>
@@ -4214,8 +4849,12 @@
       <c r="E142" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>261</v>
       </c>
@@ -4228,8 +4867,12 @@
       <c r="E143" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>69</v>
       </c>
@@ -4242,8 +4885,12 @@
       <c r="E144" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>219</v>
       </c>
@@ -4256,8 +4903,12 @@
       <c r="E145" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>192</v>
       </c>
@@ -4270,8 +4921,12 @@
       <c r="E146" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>262</v>
       </c>
@@ -4284,8 +4939,12 @@
       <c r="E147" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>70</v>
       </c>
@@ -4298,8 +4957,12 @@
       <c r="E148" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="F148">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>263</v>
       </c>
@@ -4312,8 +4975,12 @@
       <c r="E149" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>264</v>
       </c>
@@ -4326,8 +4993,12 @@
       <c r="E150" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>265</v>
       </c>
@@ -4340,8 +5011,12 @@
       <c r="E151" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="F151">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>266</v>
       </c>
@@ -4354,8 +5029,12 @@
       <c r="E152" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>267</v>
       </c>
@@ -4368,8 +5047,12 @@
       <c r="E153" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>268</v>
       </c>
@@ -4382,8 +5065,12 @@
       <c r="E154" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>269</v>
       </c>
@@ -4396,8 +5083,12 @@
       <c r="E155" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>228</v>
       </c>
@@ -4410,8 +5101,12 @@
       <c r="E156" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>270</v>
       </c>
@@ -4424,8 +5119,12 @@
       <c r="E157" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>271</v>
       </c>
@@ -4438,8 +5137,12 @@
       <c r="E158" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="F158">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>152</v>
       </c>
@@ -4452,8 +5155,12 @@
       <c r="E159" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="160" spans="1:5">
+      <c r="F159">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>272</v>
       </c>
@@ -4466,8 +5173,12 @@
       <c r="E160" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="F160">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>75</v>
       </c>
@@ -4480,8 +5191,12 @@
       <c r="E161" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="162" spans="1:5">
+      <c r="F161">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>273</v>
       </c>
@@ -4494,8 +5209,12 @@
       <c r="E162" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="163" spans="1:5">
+      <c r="F162">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>274</v>
       </c>
@@ -4505,11 +5224,18 @@
       <c r="C163" t="s">
         <v>72</v>
       </c>
+      <c r="D163" t="s">
+        <v>299</v>
+      </c>
       <c r="E163" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="164" spans="1:5">
+      <c r="F163">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>275</v>
       </c>
@@ -4522,8 +5248,12 @@
       <c r="E164" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="165" spans="1:5">
+      <c r="F164">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>276</v>
       </c>
@@ -4536,8 +5266,12 @@
       <c r="E165" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="166" spans="1:5">
+      <c r="F165">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>80</v>
       </c>
@@ -4547,11 +5281,18 @@
       <c r="C166" t="s">
         <v>72</v>
       </c>
+      <c r="D166" t="s">
+        <v>300</v>
+      </c>
       <c r="E166" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="167" spans="1:5">
+      <c r="F166">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>277</v>
       </c>
@@ -4564,8 +5305,12 @@
       <c r="E167" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="168" spans="1:5">
+      <c r="F167">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>278</v>
       </c>
@@ -4578,8 +5323,12 @@
       <c r="E168" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="169" spans="1:5">
+      <c r="F168">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>279</v>
       </c>
@@ -4589,11 +5338,18 @@
       <c r="C169" t="s">
         <v>72</v>
       </c>
+      <c r="D169" t="s">
+        <v>301</v>
+      </c>
       <c r="E169" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="170" spans="1:5">
+      <c r="F169">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>280</v>
       </c>
@@ -4606,8 +5362,12 @@
       <c r="E170" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="171" spans="1:5">
+      <c r="F170">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>82</v>
       </c>
@@ -4620,8 +5380,12 @@
       <c r="E171" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="172" spans="1:5">
+      <c r="F171">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>281</v>
       </c>
@@ -4634,8 +5398,12 @@
       <c r="E172" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="F172">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>282</v>
       </c>
@@ -4648,8 +5416,12 @@
       <c r="E173" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="174" spans="1:5">
+      <c r="F173">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>283</v>
       </c>
@@ -4662,8 +5434,12 @@
       <c r="E174" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="175" spans="1:5">
+      <c r="F174">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>284</v>
       </c>
@@ -4676,8 +5452,12 @@
       <c r="E175" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="176" spans="1:5">
+      <c r="F175">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>172</v>
       </c>
@@ -4690,8 +5470,12 @@
       <c r="E176" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="177" spans="1:5">
+      <c r="F176">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>207</v>
       </c>
@@ -4704,8 +5488,12 @@
       <c r="E177" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="178" spans="1:5">
+      <c r="F177">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>285</v>
       </c>
@@ -4718,8 +5506,12 @@
       <c r="E178" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="179" spans="1:5">
+      <c r="F178">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>286</v>
       </c>
@@ -4732,8 +5524,12 @@
       <c r="E179" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="180" spans="1:5">
+      <c r="F179">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>219</v>
       </c>
@@ -4746,8 +5542,12 @@
       <c r="E180" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="181" spans="1:5">
+      <c r="F180">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>287</v>
       </c>
@@ -4759,6 +5559,10 @@
       </c>
       <c r="E181" t="s">
         <v>16</v>
+      </c>
+      <c r="F181">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>